<commit_message>
add login menu and new music
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NMCNTTPygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB3A2FA-BE37-4A58-B1A2-C7941BB8A30D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907BEB5-00D7-4EA6-840A-C447140FC1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3736D234-788C-4AB4-8C65-977795AFA9D8}"/>
   </bookViews>
@@ -84,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,7 +93,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,7 +133,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -140,16 +146,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2192A1E8-A4FB-4096-A61F-74F98721DC13}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="L98" sqref="L98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -486,48 +501,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
         <v>2</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="10">
         <v>3</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="10">
         <v>4</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="10">
         <v>5</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2">
@@ -1050,16 +1065,2005 @@
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="7"/>
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="D23" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
       <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="3">
+        <v>45</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="3">
+        <v>47</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="3">
+        <v>55</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="3">
+        <v>57</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="3">
+        <v>59</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="4">
+        <v>61</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E63" s="4">
+        <v>1</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0</v>
+      </c>
+      <c r="G63" s="4">
+        <v>0</v>
+      </c>
+      <c r="H63" s="4">
+        <v>0</v>
+      </c>
+      <c r="I63" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="4">
+        <v>62</v>
+      </c>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E64" s="4">
+        <v>1</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0</v>
+      </c>
+      <c r="G64" s="4">
+        <v>0</v>
+      </c>
+      <c r="H64" s="4">
+        <v>0</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="4">
+        <v>63</v>
+      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E65" s="4">
+        <v>1</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0</v>
+      </c>
+      <c r="G65" s="4">
+        <v>0</v>
+      </c>
+      <c r="H65" s="4">
+        <v>0</v>
+      </c>
+      <c r="I65" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="4">
+        <v>64</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E66" s="4">
+        <v>1</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0</v>
+      </c>
+      <c r="G66" s="4">
+        <v>0</v>
+      </c>
+      <c r="H66" s="4">
+        <v>0</v>
+      </c>
+      <c r="I66" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="4">
+        <v>65</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E67" s="4">
+        <v>1</v>
+      </c>
+      <c r="F67" s="4">
+        <v>0</v>
+      </c>
+      <c r="G67" s="4">
+        <v>0</v>
+      </c>
+      <c r="H67" s="4">
+        <v>0</v>
+      </c>
+      <c r="I67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="4">
+        <v>66</v>
+      </c>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E68" s="4">
+        <v>1</v>
+      </c>
+      <c r="F68" s="4">
+        <v>0</v>
+      </c>
+      <c r="G68" s="4">
+        <v>0</v>
+      </c>
+      <c r="H68" s="4">
+        <v>0</v>
+      </c>
+      <c r="I68" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="4">
+        <v>67</v>
+      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E69" s="4">
+        <v>1</v>
+      </c>
+      <c r="F69" s="4">
+        <v>0</v>
+      </c>
+      <c r="G69" s="4">
+        <v>0</v>
+      </c>
+      <c r="H69" s="4">
+        <v>0</v>
+      </c>
+      <c r="I69" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="4">
+        <v>68</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E70" s="4">
+        <v>1</v>
+      </c>
+      <c r="F70" s="4">
+        <v>0</v>
+      </c>
+      <c r="G70" s="4">
+        <v>0</v>
+      </c>
+      <c r="H70" s="4">
+        <v>0</v>
+      </c>
+      <c r="I70" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="4">
+        <v>69</v>
+      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E71" s="4">
+        <v>1</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0</v>
+      </c>
+      <c r="G71" s="4">
+        <v>0</v>
+      </c>
+      <c r="H71" s="4">
+        <v>0</v>
+      </c>
+      <c r="I71" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="4">
+        <v>70</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E72" s="4">
+        <v>1</v>
+      </c>
+      <c r="F72" s="4">
+        <v>0</v>
+      </c>
+      <c r="G72" s="4">
+        <v>0</v>
+      </c>
+      <c r="H72" s="4">
+        <v>0</v>
+      </c>
+      <c r="I72" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="4">
+        <v>71</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E73" s="4">
+        <v>1</v>
+      </c>
+      <c r="F73" s="4">
+        <v>0</v>
+      </c>
+      <c r="G73" s="4">
+        <v>0</v>
+      </c>
+      <c r="H73" s="4">
+        <v>0</v>
+      </c>
+      <c r="I73" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="4">
+        <v>72</v>
+      </c>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E74" s="4">
+        <v>1</v>
+      </c>
+      <c r="F74" s="4">
+        <v>0</v>
+      </c>
+      <c r="G74" s="4">
+        <v>0</v>
+      </c>
+      <c r="H74" s="4">
+        <v>0</v>
+      </c>
+      <c r="I74" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="4">
+        <v>73</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E75" s="4">
+        <v>1</v>
+      </c>
+      <c r="F75" s="4">
+        <v>0</v>
+      </c>
+      <c r="G75" s="4">
+        <v>0</v>
+      </c>
+      <c r="H75" s="4">
+        <v>0</v>
+      </c>
+      <c r="I75" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="4">
+        <v>74</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E76" s="4">
+        <v>1</v>
+      </c>
+      <c r="F76" s="4">
+        <v>0</v>
+      </c>
+      <c r="G76" s="4">
+        <v>0</v>
+      </c>
+      <c r="H76" s="4">
+        <v>0</v>
+      </c>
+      <c r="I76" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="4">
+        <v>75</v>
+      </c>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E77" s="4">
+        <v>1</v>
+      </c>
+      <c r="F77" s="4">
+        <v>0</v>
+      </c>
+      <c r="G77" s="4">
+        <v>0</v>
+      </c>
+      <c r="H77" s="4">
+        <v>0</v>
+      </c>
+      <c r="I77" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="4">
+        <v>76</v>
+      </c>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E78" s="4">
+        <v>1</v>
+      </c>
+      <c r="F78" s="4">
+        <v>0</v>
+      </c>
+      <c r="G78" s="4">
+        <v>0</v>
+      </c>
+      <c r="H78" s="4">
+        <v>0</v>
+      </c>
+      <c r="I78" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="4">
+        <v>77</v>
+      </c>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E79" s="4">
+        <v>1</v>
+      </c>
+      <c r="F79" s="4">
+        <v>0</v>
+      </c>
+      <c r="G79" s="4">
+        <v>0</v>
+      </c>
+      <c r="H79" s="4">
+        <v>0</v>
+      </c>
+      <c r="I79" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="4">
+        <v>78</v>
+      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E80" s="4">
+        <v>1</v>
+      </c>
+      <c r="F80" s="4">
+        <v>0</v>
+      </c>
+      <c r="G80" s="4">
+        <v>0</v>
+      </c>
+      <c r="H80" s="4">
+        <v>0</v>
+      </c>
+      <c r="I80" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="4">
+        <v>79</v>
+      </c>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E81" s="4">
+        <v>1</v>
+      </c>
+      <c r="F81" s="4">
+        <v>0</v>
+      </c>
+      <c r="G81" s="4">
+        <v>0</v>
+      </c>
+      <c r="H81" s="4">
+        <v>0</v>
+      </c>
+      <c r="I81" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="4">
+        <v>80</v>
+      </c>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E82" s="4">
+        <v>1</v>
+      </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
+      <c r="G82" s="4">
+        <v>0</v>
+      </c>
+      <c r="H82" s="4">
+        <v>0</v>
+      </c>
+      <c r="I82" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="4">
+        <v>81</v>
+      </c>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E83" s="4">
+        <v>1</v>
+      </c>
+      <c r="F83" s="4">
+        <v>0</v>
+      </c>
+      <c r="G83" s="4">
+        <v>0</v>
+      </c>
+      <c r="H83" s="4">
+        <v>0</v>
+      </c>
+      <c r="I83" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="4">
+        <v>82</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E84" s="4">
+        <v>1</v>
+      </c>
+      <c r="F84" s="4">
+        <v>0</v>
+      </c>
+      <c r="G84" s="4">
+        <v>0</v>
+      </c>
+      <c r="H84" s="4">
+        <v>0</v>
+      </c>
+      <c r="I84" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="4">
+        <v>83</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E85" s="4">
+        <v>1</v>
+      </c>
+      <c r="F85" s="4">
+        <v>0</v>
+      </c>
+      <c r="G85" s="4">
+        <v>0</v>
+      </c>
+      <c r="H85" s="4">
+        <v>0</v>
+      </c>
+      <c r="I85" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="4">
+        <v>84</v>
+      </c>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E86" s="4">
+        <v>1</v>
+      </c>
+      <c r="F86" s="4">
+        <v>0</v>
+      </c>
+      <c r="G86" s="4">
+        <v>0</v>
+      </c>
+      <c r="H86" s="4">
+        <v>0</v>
+      </c>
+      <c r="I86" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="4">
+        <v>85</v>
+      </c>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E87" s="4">
+        <v>1</v>
+      </c>
+      <c r="F87" s="4">
+        <v>0</v>
+      </c>
+      <c r="G87" s="4">
+        <v>0</v>
+      </c>
+      <c r="H87" s="4">
+        <v>0</v>
+      </c>
+      <c r="I87" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="4">
+        <v>86</v>
+      </c>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E88" s="4">
+        <v>1</v>
+      </c>
+      <c r="F88" s="4">
+        <v>0</v>
+      </c>
+      <c r="G88" s="4">
+        <v>0</v>
+      </c>
+      <c r="H88" s="4">
+        <v>0</v>
+      </c>
+      <c r="I88" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="4">
+        <v>87</v>
+      </c>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E89" s="4">
+        <v>1</v>
+      </c>
+      <c r="F89" s="4">
+        <v>0</v>
+      </c>
+      <c r="G89" s="4">
+        <v>0</v>
+      </c>
+      <c r="H89" s="4">
+        <v>0</v>
+      </c>
+      <c r="I89" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="4">
+        <v>88</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E90" s="4">
+        <v>1</v>
+      </c>
+      <c r="F90" s="4">
+        <v>0</v>
+      </c>
+      <c r="G90" s="4">
+        <v>0</v>
+      </c>
+      <c r="H90" s="4">
+        <v>0</v>
+      </c>
+      <c r="I90" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="4">
+        <v>89</v>
+      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E91" s="4">
+        <v>1</v>
+      </c>
+      <c r="F91" s="4">
+        <v>0</v>
+      </c>
+      <c r="G91" s="4">
+        <v>0</v>
+      </c>
+      <c r="H91" s="4">
+        <v>0</v>
+      </c>
+      <c r="I91" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="4">
+        <v>90</v>
+      </c>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E92" s="4">
+        <v>1</v>
+      </c>
+      <c r="F92" s="4">
+        <v>0</v>
+      </c>
+      <c r="G92" s="4">
+        <v>0</v>
+      </c>
+      <c r="H92" s="4">
+        <v>0</v>
+      </c>
+      <c r="I92" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="4">
+        <v>91</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E93" s="4">
+        <v>1</v>
+      </c>
+      <c r="F93" s="4">
+        <v>0</v>
+      </c>
+      <c r="G93" s="4">
+        <v>0</v>
+      </c>
+      <c r="H93" s="4">
+        <v>0</v>
+      </c>
+      <c r="I93" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="4">
+        <v>92</v>
+      </c>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E94" s="4">
+        <v>1</v>
+      </c>
+      <c r="F94" s="4">
+        <v>0</v>
+      </c>
+      <c r="G94" s="4">
+        <v>0</v>
+      </c>
+      <c r="H94" s="4">
+        <v>0</v>
+      </c>
+      <c r="I94" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="4">
+        <v>93</v>
+      </c>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E95" s="4">
+        <v>1</v>
+      </c>
+      <c r="F95" s="4">
+        <v>0</v>
+      </c>
+      <c r="G95" s="4">
+        <v>0</v>
+      </c>
+      <c r="H95" s="4">
+        <v>0</v>
+      </c>
+      <c r="I95" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="4">
+        <v>94</v>
+      </c>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E96" s="4">
+        <v>1</v>
+      </c>
+      <c r="F96" s="4">
+        <v>0</v>
+      </c>
+      <c r="G96" s="4">
+        <v>0</v>
+      </c>
+      <c r="H96" s="4">
+        <v>0</v>
+      </c>
+      <c r="I96" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="4">
+        <v>95</v>
+      </c>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E97" s="4">
+        <v>1</v>
+      </c>
+      <c r="F97" s="4">
+        <v>0</v>
+      </c>
+      <c r="G97" s="4">
+        <v>0</v>
+      </c>
+      <c r="H97" s="4">
+        <v>0</v>
+      </c>
+      <c r="I97" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="4">
+        <v>96</v>
+      </c>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E98" s="4">
+        <v>1</v>
+      </c>
+      <c r="F98" s="4">
+        <v>0</v>
+      </c>
+      <c r="G98" s="4">
+        <v>0</v>
+      </c>
+      <c r="H98" s="4">
+        <v>0</v>
+      </c>
+      <c r="I98" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="4">
+        <v>97</v>
+      </c>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E99" s="4">
+        <v>1</v>
+      </c>
+      <c r="F99" s="4">
+        <v>0</v>
+      </c>
+      <c r="G99" s="4">
+        <v>0</v>
+      </c>
+      <c r="H99" s="4">
+        <v>0</v>
+      </c>
+      <c r="I99" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="4">
+        <v>98</v>
+      </c>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E100" s="4">
+        <v>1</v>
+      </c>
+      <c r="F100" s="4">
+        <v>0</v>
+      </c>
+      <c r="G100" s="4">
+        <v>0</v>
+      </c>
+      <c r="H100" s="4">
+        <v>0</v>
+      </c>
+      <c r="I100" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="4">
+        <v>99</v>
+      </c>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E101" s="4">
+        <v>1</v>
+      </c>
+      <c r="F101" s="4">
+        <v>0</v>
+      </c>
+      <c r="G101" s="4">
+        <v>0</v>
+      </c>
+      <c r="H101" s="4">
+        <v>0</v>
+      </c>
+      <c r="I101" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="4">
+        <v>100</v>
+      </c>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E102" s="4">
+        <v>1</v>
+      </c>
+      <c r="F102" s="4">
+        <v>0</v>
+      </c>
+      <c r="G102" s="4">
+        <v>0</v>
+      </c>
+      <c r="H102" s="4">
+        <v>0</v>
+      </c>
+      <c r="I102" s="4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>